<commit_message>
XGBoost model 1 SMOTE 4000
</commit_message>
<xml_diff>
--- a/Data/Predictions/Logistic Regression/smote_rating_change_model_1/smote_rating_change_model_1_predictions.xlsx
+++ b/Data/Predictions/Logistic Regression/smote_rating_change_model_1/smote_rating_change_model_1_predictions.xlsx
@@ -475,7 +475,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -535,7 +535,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -675,7 +675,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -715,7 +715,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -755,7 +755,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -775,7 +775,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -795,7 +795,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -835,7 +835,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -855,7 +855,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -895,7 +895,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -935,7 +935,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -955,7 +955,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -975,7 +975,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -995,7 +995,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1135,7 +1135,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1295,7 +1295,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1535,7 +1535,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1555,7 +1555,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1615,7 +1615,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1695,7 +1695,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1715,7 +1715,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1735,7 +1735,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1755,7 +1755,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1775,7 +1775,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1995,7 +1995,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2015,7 +2015,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2135,7 +2135,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2195,7 +2195,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2215,7 +2215,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2315,7 +2315,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2335,7 +2335,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2415,7 +2415,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2435,7 +2435,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2455,7 +2455,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2515,7 +2515,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2535,7 +2535,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2575,7 +2575,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2595,7 +2595,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2615,7 +2615,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2655,7 +2655,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2675,7 +2675,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2695,7 +2695,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2715,7 +2715,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2915,7 +2915,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2935,7 +2935,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2955,7 +2955,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2995,7 +2995,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3035,7 +3035,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3055,7 +3055,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3075,7 +3075,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3095,7 +3095,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3355,7 +3355,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3595,7 +3595,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3775,7 +3775,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3795,7 +3795,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3835,7 +3835,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3995,7 +3995,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4035,7 +4035,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4075,7 +4075,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4095,7 +4095,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4115,7 +4115,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4135,7 +4135,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4175,7 +4175,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4315,7 +4315,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4335,7 +4335,7 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4355,7 +4355,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4435,7 +4435,7 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4455,7 +4455,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4635,7 +4635,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4655,7 +4655,7 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4675,7 +4675,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4695,7 +4695,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5035,7 +5035,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5055,7 +5055,7 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5075,7 +5075,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5115,7 +5115,7 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5135,7 +5135,7 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5175,7 +5175,7 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5215,7 +5215,7 @@
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5235,7 +5235,7 @@
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5255,7 +5255,7 @@
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5275,7 +5275,7 @@
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5295,7 +5295,7 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5315,7 +5315,7 @@
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5335,7 +5335,7 @@
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5355,7 +5355,7 @@
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5655,7 +5655,7 @@
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5675,7 +5675,7 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5695,7 +5695,7 @@
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5715,7 +5715,7 @@
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5735,7 +5735,7 @@
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5755,7 +5755,7 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5775,7 +5775,7 @@
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5855,7 +5855,7 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5875,7 +5875,7 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5895,7 +5895,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5935,7 +5935,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6035,7 +6035,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6055,7 +6055,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6075,7 +6075,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6095,7 +6095,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6115,7 +6115,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6135,7 +6135,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6155,7 +6155,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6175,7 +6175,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6215,7 +6215,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6235,7 +6235,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6255,7 +6255,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6275,7 +6275,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6295,7 +6295,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6315,7 +6315,7 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6355,7 +6355,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6535,7 +6535,7 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6575,7 +6575,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6595,7 +6595,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6795,7 +6795,7 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6815,7 +6815,7 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6975,7 +6975,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7035,7 +7035,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7055,7 +7055,7 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7075,7 +7075,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7095,7 +7095,7 @@
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7175,7 +7175,7 @@
       </c>
       <c r="D337" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7195,7 +7195,7 @@
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7215,7 +7215,7 @@
       </c>
       <c r="D339" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7235,7 +7235,7 @@
       </c>
       <c r="D340" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7275,7 +7275,7 @@
       </c>
       <c r="D342" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7295,7 +7295,7 @@
       </c>
       <c r="D343" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7315,7 +7315,7 @@
       </c>
       <c r="D344" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7335,7 +7335,7 @@
       </c>
       <c r="D345" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7355,7 +7355,7 @@
       </c>
       <c r="D346" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7375,7 +7375,7 @@
       </c>
       <c r="D347" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7395,7 +7395,7 @@
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7415,7 +7415,7 @@
       </c>
       <c r="D349" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7435,7 +7435,7 @@
       </c>
       <c r="D350" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7455,7 +7455,7 @@
       </c>
       <c r="D351" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7475,7 +7475,7 @@
       </c>
       <c r="D352" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7515,7 +7515,7 @@
       </c>
       <c r="D354" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7535,7 +7535,7 @@
       </c>
       <c r="D355" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7695,7 +7695,7 @@
       </c>
       <c r="D363" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7815,7 +7815,7 @@
       </c>
       <c r="D369" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7835,7 +7835,7 @@
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7855,7 +7855,7 @@
       </c>
       <c r="D371" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7875,7 +7875,7 @@
       </c>
       <c r="D372" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8155,7 +8155,7 @@
       </c>
       <c r="D386" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8175,7 +8175,7 @@
       </c>
       <c r="D387" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8335,7 +8335,7 @@
       </c>
       <c r="D395" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8355,7 +8355,7 @@
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8375,7 +8375,7 @@
       </c>
       <c r="D397" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8395,7 +8395,7 @@
       </c>
       <c r="D398" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8415,7 +8415,7 @@
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8435,7 +8435,7 @@
       </c>
       <c r="D400" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8455,7 +8455,7 @@
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8475,7 +8475,7 @@
       </c>
       <c r="D402" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8555,7 +8555,7 @@
       </c>
       <c r="D406" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8575,7 +8575,7 @@
       </c>
       <c r="D407" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8595,7 +8595,7 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8615,7 +8615,7 @@
       </c>
       <c r="D409" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8635,7 +8635,7 @@
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8655,7 +8655,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8675,7 +8675,7 @@
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8695,7 +8695,7 @@
       </c>
       <c r="D413" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8715,7 +8715,7 @@
       </c>
       <c r="D414" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8735,7 +8735,7 @@
       </c>
       <c r="D415" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8755,7 +8755,7 @@
       </c>
       <c r="D416" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8775,7 +8775,7 @@
       </c>
       <c r="D417" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9035,7 +9035,7 @@
       </c>
       <c r="D430" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9055,7 +9055,7 @@
       </c>
       <c r="D431" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9235,7 +9235,7 @@
       </c>
       <c r="D440" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9255,7 +9255,7 @@
       </c>
       <c r="D441" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9295,7 +9295,7 @@
       </c>
       <c r="D443" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9315,7 +9315,7 @@
       </c>
       <c r="D444" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9415,7 +9415,7 @@
       </c>
       <c r="D449" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9435,7 +9435,7 @@
       </c>
       <c r="D450" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9455,7 +9455,7 @@
       </c>
       <c r="D451" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9475,7 +9475,7 @@
       </c>
       <c r="D452" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9535,7 +9535,7 @@
       </c>
       <c r="D455" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9575,7 +9575,7 @@
       </c>
       <c r="D457" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9635,7 +9635,7 @@
       </c>
       <c r="D460" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9655,7 +9655,7 @@
       </c>
       <c r="D461" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9675,7 +9675,7 @@
       </c>
       <c r="D462" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9715,7 +9715,7 @@
       </c>
       <c r="D464" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9755,7 +9755,7 @@
       </c>
       <c r="D466" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9775,7 +9775,7 @@
       </c>
       <c r="D467" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9795,7 +9795,7 @@
       </c>
       <c r="D468" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9875,7 +9875,7 @@
       </c>
       <c r="D472" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9995,7 +9995,7 @@
       </c>
       <c r="D478" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10135,7 +10135,7 @@
       </c>
       <c r="D485" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10155,7 +10155,7 @@
       </c>
       <c r="D486" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10175,7 +10175,7 @@
       </c>
       <c r="D487" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10195,7 +10195,7 @@
       </c>
       <c r="D488" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10215,7 +10215,7 @@
       </c>
       <c r="D489" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10235,7 +10235,7 @@
       </c>
       <c r="D490" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10255,7 +10255,7 @@
       </c>
       <c r="D491" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10275,7 +10275,7 @@
       </c>
       <c r="D492" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10295,7 +10295,7 @@
       </c>
       <c r="D493" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10315,7 +10315,7 @@
       </c>
       <c r="D494" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10435,7 +10435,7 @@
       </c>
       <c r="D500" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10455,7 +10455,7 @@
       </c>
       <c r="D501" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10475,7 +10475,7 @@
       </c>
       <c r="D502" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10495,7 +10495,7 @@
       </c>
       <c r="D503" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10515,7 +10515,7 @@
       </c>
       <c r="D504" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10755,7 +10755,7 @@
       </c>
       <c r="D516" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10815,7 +10815,7 @@
       </c>
       <c r="D519" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10835,7 +10835,7 @@
       </c>
       <c r="D520" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10855,7 +10855,7 @@
       </c>
       <c r="D521" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10875,7 +10875,7 @@
       </c>
       <c r="D522" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10975,7 +10975,7 @@
       </c>
       <c r="D527" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10995,7 +10995,7 @@
       </c>
       <c r="D528" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11035,7 +11035,7 @@
       </c>
       <c r="D530" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11115,7 +11115,7 @@
       </c>
       <c r="D534" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11155,7 +11155,7 @@
       </c>
       <c r="D536" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11175,7 +11175,7 @@
       </c>
       <c r="D537" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11215,7 +11215,7 @@
       </c>
       <c r="D539" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11235,7 +11235,7 @@
       </c>
       <c r="D540" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11255,7 +11255,7 @@
       </c>
       <c r="D541" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11275,7 +11275,7 @@
       </c>
       <c r="D542" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11315,7 +11315,7 @@
       </c>
       <c r="D544" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11415,7 +11415,7 @@
       </c>
       <c r="D549" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11455,7 +11455,7 @@
       </c>
       <c r="D551" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11475,7 +11475,7 @@
       </c>
       <c r="D552" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11495,7 +11495,7 @@
       </c>
       <c r="D553" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11515,7 +11515,7 @@
       </c>
       <c r="D554" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11535,7 +11535,7 @@
       </c>
       <c r="D555" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11875,7 +11875,7 @@
       </c>
       <c r="D572" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11895,7 +11895,7 @@
       </c>
       <c r="D573" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11915,7 +11915,7 @@
       </c>
       <c r="D574" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11935,7 +11935,7 @@
       </c>
       <c r="D575" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12015,7 +12015,7 @@
       </c>
       <c r="D579" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12075,7 +12075,7 @@
       </c>
       <c r="D582" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12095,7 +12095,7 @@
       </c>
       <c r="D583" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12115,7 +12115,7 @@
       </c>
       <c r="D584" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12135,7 +12135,7 @@
       </c>
       <c r="D585" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12295,7 +12295,7 @@
       </c>
       <c r="D593" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12315,7 +12315,7 @@
       </c>
       <c r="D594" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12335,7 +12335,7 @@
       </c>
       <c r="D595" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12355,7 +12355,7 @@
       </c>
       <c r="D596" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12375,7 +12375,7 @@
       </c>
       <c r="D597" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12395,7 +12395,7 @@
       </c>
       <c r="D598" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12475,7 +12475,7 @@
       </c>
       <c r="D602" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12535,7 +12535,7 @@
       </c>
       <c r="D605" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12555,7 +12555,7 @@
       </c>
       <c r="D606" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12575,7 +12575,7 @@
       </c>
       <c r="D607" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12595,7 +12595,7 @@
       </c>
       <c r="D608" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12615,7 +12615,7 @@
       </c>
       <c r="D609" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12635,7 +12635,7 @@
       </c>
       <c r="D610" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12655,7 +12655,7 @@
       </c>
       <c r="D611" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12675,7 +12675,7 @@
       </c>
       <c r="D612" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12695,7 +12695,7 @@
       </c>
       <c r="D613" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12715,7 +12715,7 @@
       </c>
       <c r="D614" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12735,7 +12735,7 @@
       </c>
       <c r="D615" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12755,7 +12755,7 @@
       </c>
       <c r="D616" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13015,7 +13015,7 @@
       </c>
       <c r="D629" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13035,7 +13035,7 @@
       </c>
       <c r="D630" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13055,7 +13055,7 @@
       </c>
       <c r="D631" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13135,7 +13135,7 @@
       </c>
       <c r="D635" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13155,7 +13155,7 @@
       </c>
       <c r="D636" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13175,7 +13175,7 @@
       </c>
       <c r="D637" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13195,7 +13195,7 @@
       </c>
       <c r="D638" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13215,7 +13215,7 @@
       </c>
       <c r="D639" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13255,7 +13255,7 @@
       </c>
       <c r="D641" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13295,7 +13295,7 @@
       </c>
       <c r="D643" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13315,7 +13315,7 @@
       </c>
       <c r="D644" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13335,7 +13335,7 @@
       </c>
       <c r="D645" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13375,7 +13375,7 @@
       </c>
       <c r="D647" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13395,7 +13395,7 @@
       </c>
       <c r="D648" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13415,7 +13415,7 @@
       </c>
       <c r="D649" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13455,7 +13455,7 @@
       </c>
       <c r="D651" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13515,7 +13515,7 @@
       </c>
       <c r="D654" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13595,7 +13595,7 @@
       </c>
       <c r="D658" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13615,7 +13615,7 @@
       </c>
       <c r="D659" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13635,7 +13635,7 @@
       </c>
       <c r="D660" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13655,7 +13655,7 @@
       </c>
       <c r="D661" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13735,7 +13735,7 @@
       </c>
       <c r="D665" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13755,7 +13755,7 @@
       </c>
       <c r="D666" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13775,7 +13775,7 @@
       </c>
       <c r="D667" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13815,7 +13815,7 @@
       </c>
       <c r="D669" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13835,7 +13835,7 @@
       </c>
       <c r="D670" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13875,7 +13875,7 @@
       </c>
       <c r="D672" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14035,7 +14035,7 @@
       </c>
       <c r="D680" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14215,7 +14215,7 @@
       </c>
       <c r="D689" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14395,7 +14395,7 @@
       </c>
       <c r="D698" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14495,7 +14495,7 @@
       </c>
       <c r="D703" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14515,7 +14515,7 @@
       </c>
       <c r="D704" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14535,7 +14535,7 @@
       </c>
       <c r="D705" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14555,7 +14555,7 @@
       </c>
       <c r="D706" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14575,7 +14575,7 @@
       </c>
       <c r="D707" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14675,7 +14675,7 @@
       </c>
       <c r="D712" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14695,7 +14695,7 @@
       </c>
       <c r="D713" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14715,7 +14715,7 @@
       </c>
       <c r="D714" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14735,7 +14735,7 @@
       </c>
       <c r="D715" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14795,7 +14795,7 @@
       </c>
       <c r="D718" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14895,7 +14895,7 @@
       </c>
       <c r="D723" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14915,7 +14915,7 @@
       </c>
       <c r="D724" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14955,7 +14955,7 @@
       </c>
       <c r="D726" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15155,7 +15155,7 @@
       </c>
       <c r="D736" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15175,7 +15175,7 @@
       </c>
       <c r="D737" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15255,7 +15255,7 @@
       </c>
       <c r="D741" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15275,7 +15275,7 @@
       </c>
       <c r="D742" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15315,7 +15315,7 @@
       </c>
       <c r="D744" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15395,7 +15395,7 @@
       </c>
       <c r="D748" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15475,7 +15475,7 @@
       </c>
       <c r="D752" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15575,7 +15575,7 @@
       </c>
       <c r="D757" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15595,7 +15595,7 @@
       </c>
       <c r="D758" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15615,7 +15615,7 @@
       </c>
       <c r="D759" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15635,7 +15635,7 @@
       </c>
       <c r="D760" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15655,7 +15655,7 @@
       </c>
       <c r="D761" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15695,7 +15695,7 @@
       </c>
       <c r="D763" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15715,7 +15715,7 @@
       </c>
       <c r="D764" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15735,7 +15735,7 @@
       </c>
       <c r="D765" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15755,7 +15755,7 @@
       </c>
       <c r="D766" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15775,7 +15775,7 @@
       </c>
       <c r="D767" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15795,7 +15795,7 @@
       </c>
       <c r="D768" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15815,7 +15815,7 @@
       </c>
       <c r="D769" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15835,7 +15835,7 @@
       </c>
       <c r="D770" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15935,7 +15935,7 @@
       </c>
       <c r="D775" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16355,7 +16355,7 @@
       </c>
       <c r="D796" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16435,7 +16435,7 @@
       </c>
       <c r="D800" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16495,7 +16495,7 @@
       </c>
       <c r="D803" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16575,7 +16575,7 @@
       </c>
       <c r="D807" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16595,7 +16595,7 @@
       </c>
       <c r="D808" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16615,7 +16615,7 @@
       </c>
       <c r="D809" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16635,7 +16635,7 @@
       </c>
       <c r="D810" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16655,7 +16655,7 @@
       </c>
       <c r="D811" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16675,7 +16675,7 @@
       </c>
       <c r="D812" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16695,7 +16695,7 @@
       </c>
       <c r="D813" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16715,7 +16715,7 @@
       </c>
       <c r="D814" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16755,7 +16755,7 @@
       </c>
       <c r="D816" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16775,7 +16775,7 @@
       </c>
       <c r="D817" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16855,7 +16855,7 @@
       </c>
       <c r="D821" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16875,7 +16875,7 @@
       </c>
       <c r="D822" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16895,7 +16895,7 @@
       </c>
       <c r="D823" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16935,7 +16935,7 @@
       </c>
       <c r="D825" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16955,7 +16955,7 @@
       </c>
       <c r="D826" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16975,7 +16975,7 @@
       </c>
       <c r="D827" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16995,7 +16995,7 @@
       </c>
       <c r="D828" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17015,7 +17015,7 @@
       </c>
       <c r="D829" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17395,7 +17395,7 @@
       </c>
       <c r="D848" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17415,7 +17415,7 @@
       </c>
       <c r="D849" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17515,7 +17515,7 @@
       </c>
       <c r="D854" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17535,7 +17535,7 @@
       </c>
       <c r="D855" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17775,7 +17775,7 @@
       </c>
       <c r="D867" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17795,7 +17795,7 @@
       </c>
       <c r="D868" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17815,7 +17815,7 @@
       </c>
       <c r="D869" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17835,7 +17835,7 @@
       </c>
       <c r="D870" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17855,7 +17855,7 @@
       </c>
       <c r="D871" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17875,7 +17875,7 @@
       </c>
       <c r="D872" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17895,7 +17895,7 @@
       </c>
       <c r="D873" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17915,7 +17915,7 @@
       </c>
       <c r="D874" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17935,7 +17935,7 @@
       </c>
       <c r="D875" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17955,7 +17955,7 @@
       </c>
       <c r="D876" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17995,7 +17995,7 @@
       </c>
       <c r="D878" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18015,7 +18015,7 @@
       </c>
       <c r="D879" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18035,7 +18035,7 @@
       </c>
       <c r="D880" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18055,7 +18055,7 @@
       </c>
       <c r="D881" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18075,7 +18075,7 @@
       </c>
       <c r="D882" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18095,7 +18095,7 @@
       </c>
       <c r="D883" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18155,7 +18155,7 @@
       </c>
       <c r="D886" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18455,7 +18455,7 @@
       </c>
       <c r="D901" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18595,7 +18595,7 @@
       </c>
       <c r="D908" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18615,7 +18615,7 @@
       </c>
       <c r="D909" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18635,7 +18635,7 @@
       </c>
       <c r="D910" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18655,7 +18655,7 @@
       </c>
       <c r="D911" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18675,7 +18675,7 @@
       </c>
       <c r="D912" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18695,7 +18695,7 @@
       </c>
       <c r="D913" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18735,7 +18735,7 @@
       </c>
       <c r="D915" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18755,7 +18755,7 @@
       </c>
       <c r="D916" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18875,7 +18875,7 @@
       </c>
       <c r="D922" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18895,7 +18895,7 @@
       </c>
       <c r="D923" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18915,7 +18915,7 @@
       </c>
       <c r="D924" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18975,7 +18975,7 @@
       </c>
       <c r="D927" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19055,7 +19055,7 @@
       </c>
       <c r="D931" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19075,7 +19075,7 @@
       </c>
       <c r="D932" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19095,7 +19095,7 @@
       </c>
       <c r="D933" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19115,7 +19115,7 @@
       </c>
       <c r="D934" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19135,7 +19135,7 @@
       </c>
       <c r="D935" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19155,7 +19155,7 @@
       </c>
       <c r="D936" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19175,7 +19175,7 @@
       </c>
       <c r="D937" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19195,7 +19195,7 @@
       </c>
       <c r="D938" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19255,7 +19255,7 @@
       </c>
       <c r="D941" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19275,7 +19275,7 @@
       </c>
       <c r="D942" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19295,7 +19295,7 @@
       </c>
       <c r="D943" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19315,7 +19315,7 @@
       </c>
       <c r="D944" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19335,7 +19335,7 @@
       </c>
       <c r="D945" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19375,7 +19375,7 @@
       </c>
       <c r="D947" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19415,7 +19415,7 @@
       </c>
       <c r="D949" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19475,7 +19475,7 @@
       </c>
       <c r="D952" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19535,7 +19535,7 @@
       </c>
       <c r="D955" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19555,7 +19555,7 @@
       </c>
       <c r="D956" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19575,7 +19575,7 @@
       </c>
       <c r="D957" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19615,7 +19615,7 @@
       </c>
       <c r="D959" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19635,7 +19635,7 @@
       </c>
       <c r="D960" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19655,7 +19655,7 @@
       </c>
       <c r="D961" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19815,7 +19815,7 @@
       </c>
       <c r="D969" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19915,7 +19915,7 @@
       </c>
       <c r="D974" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19935,7 +19935,7 @@
       </c>
       <c r="D975" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19955,7 +19955,7 @@
       </c>
       <c r="D976" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19975,7 +19975,7 @@
       </c>
       <c r="D977" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19995,7 +19995,7 @@
       </c>
       <c r="D978" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20195,7 +20195,7 @@
       </c>
       <c r="D988" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20215,7 +20215,7 @@
       </c>
       <c r="D989" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20595,7 +20595,7 @@
       </c>
       <c r="D1008" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20635,7 +20635,7 @@
       </c>
       <c r="D1010" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20655,7 +20655,7 @@
       </c>
       <c r="D1011" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20675,7 +20675,7 @@
       </c>
       <c r="D1012" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20695,7 +20695,7 @@
       </c>
       <c r="D1013" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20715,7 +20715,7 @@
       </c>
       <c r="D1014" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20735,7 +20735,7 @@
       </c>
       <c r="D1015" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20775,7 +20775,7 @@
       </c>
       <c r="D1017" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20795,7 +20795,7 @@
       </c>
       <c r="D1018" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20875,7 +20875,7 @@
       </c>
       <c r="D1022" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20995,7 +20995,7 @@
       </c>
       <c r="D1028" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21015,7 +21015,7 @@
       </c>
       <c r="D1029" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21115,7 +21115,7 @@
       </c>
       <c r="D1034" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21135,7 +21135,7 @@
       </c>
       <c r="D1035" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21155,7 +21155,7 @@
       </c>
       <c r="D1036" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21175,7 +21175,7 @@
       </c>
       <c r="D1037" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21235,7 +21235,7 @@
       </c>
       <c r="D1040" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21255,7 +21255,7 @@
       </c>
       <c r="D1041" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21295,7 +21295,7 @@
       </c>
       <c r="D1043" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21355,7 +21355,7 @@
       </c>
       <c r="D1046" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21375,7 +21375,7 @@
       </c>
       <c r="D1047" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21395,7 +21395,7 @@
       </c>
       <c r="D1048" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21555,7 +21555,7 @@
       </c>
       <c r="D1056" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21575,7 +21575,7 @@
       </c>
       <c r="D1057" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21595,7 +21595,7 @@
       </c>
       <c r="D1058" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21615,7 +21615,7 @@
       </c>
       <c r="D1059" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21635,7 +21635,7 @@
       </c>
       <c r="D1060" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21835,7 +21835,7 @@
       </c>
       <c r="D1070" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21855,7 +21855,7 @@
       </c>
       <c r="D1071" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21975,7 +21975,7 @@
       </c>
       <c r="D1077" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21995,7 +21995,7 @@
       </c>
       <c r="D1078" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22015,7 +22015,7 @@
       </c>
       <c r="D1079" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22035,7 +22035,7 @@
       </c>
       <c r="D1080" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22055,7 +22055,7 @@
       </c>
       <c r="D1081" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22095,7 +22095,7 @@
       </c>
       <c r="D1083" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22115,7 +22115,7 @@
       </c>
       <c r="D1084" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22135,7 +22135,7 @@
       </c>
       <c r="D1085" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22235,7 +22235,7 @@
       </c>
       <c r="D1090" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22255,7 +22255,7 @@
       </c>
       <c r="D1091" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22275,7 +22275,7 @@
       </c>
       <c r="D1092" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22295,7 +22295,7 @@
       </c>
       <c r="D1093" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22315,7 +22315,7 @@
       </c>
       <c r="D1094" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22475,7 +22475,7 @@
       </c>
       <c r="D1102" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22695,7 +22695,7 @@
       </c>
       <c r="D1113" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22715,7 +22715,7 @@
       </c>
       <c r="D1114" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22735,7 +22735,7 @@
       </c>
       <c r="D1115" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22755,7 +22755,7 @@
       </c>
       <c r="D1116" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22795,7 +22795,7 @@
       </c>
       <c r="D1118" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22815,7 +22815,7 @@
       </c>
       <c r="D1119" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Logistic Change Model 1 update output
</commit_message>
<xml_diff>
--- a/Data/Predictions/Logistic Regression/smote_rating_change_model_1/smote_rating_change_model_1_predictions.xlsx
+++ b/Data/Predictions/Logistic Regression/smote_rating_change_model_1/smote_rating_change_model_1_predictions.xlsx
@@ -1115,7 +1115,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1135,7 +1135,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2715,7 +2715,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2875,7 +2875,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3575,7 +3575,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3715,7 +3715,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4275,7 +4275,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4515,7 +4515,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4955,7 +4955,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6055,7 +6055,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6255,7 +6255,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6375,7 +6375,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6415,7 +6415,7 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6775,7 +6775,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6875,7 +6875,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7995,7 +7995,7 @@
       </c>
       <c r="D378" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8555,7 +8555,7 @@
       </c>
       <c r="D406" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8575,7 +8575,7 @@
       </c>
       <c r="D407" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8715,7 +8715,7 @@
       </c>
       <c r="D414" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8935,7 +8935,7 @@
       </c>
       <c r="D425" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9015,7 +9015,7 @@
       </c>
       <c r="D429" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9735,7 +9735,7 @@
       </c>
       <c r="D465" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9935,7 +9935,7 @@
       </c>
       <c r="D475" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10155,7 +10155,7 @@
       </c>
       <c r="D486" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10375,7 +10375,7 @@
       </c>
       <c r="D497" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10555,7 +10555,7 @@
       </c>
       <c r="D506" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11335,7 +11335,7 @@
       </c>
       <c r="D545" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11535,7 +11535,7 @@
       </c>
       <c r="D555" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11735,7 +11735,7 @@
       </c>
       <c r="D565" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11795,7 +11795,7 @@
       </c>
       <c r="D568" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12255,7 +12255,7 @@
       </c>
       <c r="D591" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12395,7 +12395,7 @@
       </c>
       <c r="D598" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12415,7 +12415,7 @@
       </c>
       <c r="D599" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12875,7 +12875,7 @@
       </c>
       <c r="D622" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13155,7 +13155,7 @@
       </c>
       <c r="D636" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13295,7 +13295,7 @@
       </c>
       <c r="D643" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13475,7 +13475,7 @@
       </c>
       <c r="D652" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14195,7 +14195,7 @@
       </c>
       <c r="D688" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14655,7 +14655,7 @@
       </c>
       <c r="D711" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14775,7 +14775,7 @@
       </c>
       <c r="D717" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15275,7 +15275,7 @@
       </c>
       <c r="D742" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15295,7 +15295,7 @@
       </c>
       <c r="D743" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15415,7 +15415,7 @@
       </c>
       <c r="D749" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15715,7 +15715,7 @@
       </c>
       <c r="D764" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15735,7 +15735,7 @@
       </c>
       <c r="D765" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16455,7 +16455,7 @@
       </c>
       <c r="D801" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18155,7 +18155,7 @@
       </c>
       <c r="D886" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19735,7 +19735,7 @@
       </c>
       <c r="D965" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20355,7 +20355,7 @@
       </c>
       <c r="D996" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20655,7 +20655,7 @@
       </c>
       <c r="D1011" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20755,7 +20755,7 @@
       </c>
       <c r="D1016" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21055,7 +21055,7 @@
       </c>
       <c r="D1031" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21455,7 +21455,7 @@
       </c>
       <c r="D1051" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21635,7 +21635,7 @@
       </c>
       <c r="D1060" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21795,7 +21795,7 @@
       </c>
       <c r="D1068" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22375,7 +22375,7 @@
       </c>
       <c r="D1097" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22755,7 +22755,7 @@
       </c>
       <c r="D1116" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22795,7 +22795,7 @@
       </c>
       <c r="D1118" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>

</xml_diff>